<commit_message>
Se agrega la funcionalidades de borrados con sp de perfiles y de grados clasif
</commit_message>
<xml_diff>
--- a/cotto-system/Plantillas/plantilla_carga_gradosclasif1.xlsx
+++ b/cotto-system/Plantillas/plantilla_carga_gradosclasif1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2132" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135" uniqueCount="172">
   <si>
     <t>gradocolor</t>
   </si>
@@ -532,6 +532,15 @@
   <si>
     <t>31-3</t>
   </si>
+  <si>
+    <t>Moy</t>
+  </si>
+  <si>
+    <t>Guerrrero</t>
+  </si>
+  <si>
+    <t>Vazquez</t>
+  </si>
 </sst>
 </file>
 
@@ -868,7 +877,7 @@
   <dimension ref="A1:D1281"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,6 +909,9 @@
       <c r="B2" s="1">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>169</v>
+      </c>
       <c r="D2" s="1">
         <v>1</v>
       </c>
@@ -911,6 +923,9 @@
       <c r="B3" s="1">
         <v>2</v>
       </c>
+      <c r="C3" t="s">
+        <v>170</v>
+      </c>
       <c r="D3" s="1">
         <v>1</v>
       </c>
@@ -921,6 +936,9 @@
       </c>
       <c r="B4" s="1">
         <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>171</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>

</xml_diff>